<commit_message>
Changed place risk to a double precision number. Set place risk to ~0.1 for current "no risk" activities. Flipped the processing order of the probabilities in the Person chooseOne method for speed.
git-svn-id: https://scrap.dis.anl.gov/repos/MRSA/models/agentmodel@233 eb7698ad-c3c5-4393-a60c-5d690fe7bf3d
</commit_message>
<xml_diff>
--- a/MRSA/MRSA Parameters.xlsx
+++ b/MRSA/MRSA Parameters.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Range Factor</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Checks</t>
+  </si>
+  <si>
+    <t>No Change, So OK</t>
   </si>
 </sst>
 </file>
@@ -72,8 +75,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="0.00000E+00"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.00000E+00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -138,7 +141,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -166,8 +169,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,14 +191,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="39">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -197,6 +213,12 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -209,6 +231,12 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -463,11 +491,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:hiLowLines/>
-        <c:axId val="792354024"/>
-        <c:axId val="792576216"/>
+        <c:axId val="2075435016"/>
+        <c:axId val="2075375608"/>
       </c:stockChart>
       <c:catAx>
-        <c:axId val="792354024"/>
+        <c:axId val="2075435016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -476,7 +504,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="792576216"/>
+        <c:crossAx val="2075375608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -484,7 +512,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="792576216"/>
+        <c:axId val="2075375608"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -497,7 +525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="792354024"/>
+        <c:crossAx val="2075435016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -871,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:K7"/>
+  <dimension ref="C1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:G1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17:R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1073,6 +1101,70 @@
       <c r="K7" s="3" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="15:18">
+      <c r="O17" t="s">
+        <v>6</v>
+      </c>
+      <c r="P17" s="8">
+        <v>3.1446700000000002E-4</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>6.8527000000000003E-5</v>
+      </c>
+      <c r="R17" s="8">
+        <v>7.0121599999999995E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="15:18">
+      <c r="O18" t="s">
+        <v>7</v>
+      </c>
+      <c r="P18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="15:18">
+      <c r="O19" t="s">
+        <v>8</v>
+      </c>
+      <c r="P19" s="8">
+        <v>1.3314699999999999E-4</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>2.37945E-3</v>
+      </c>
+      <c r="R19" s="8">
+        <v>6.8397900000000003E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="15:18">
+      <c r="O20" t="s">
+        <v>9</v>
+      </c>
+      <c r="P20" s="8">
+        <v>3.1500500000000002E-3</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>2.6753200000000001E-2</v>
+      </c>
+      <c r="R20" s="8">
+        <v>6.6541300000000003E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="15:18">
+      <c r="O21" t="s">
+        <v>10</v>
+      </c>
+      <c r="P21" s="8">
+        <v>6.1818199999999997E-5</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>5.8311699999999999E-5</v>
+      </c>
+      <c r="R21" s="8">
+        <v>1.5783099999999999E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>